<commit_message>
Desarrollo Vista Pg quienes somos
</commit_message>
<xml_diff>
--- a/Documentacion/Product_Backlog.xlsx
+++ b/Documentacion/Product_Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalan\Desktop\ProyectoCiclo4\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D3FBC4-ED39-4955-A94F-9AB79C7CDACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05DA99B-96A9-4D02-9F73-4D6D48A76422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="11760" windowHeight="20130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog34.8" sheetId="3" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>Desarrollo Vista Pagina Detalle Producto</t>
   </si>
   <si>
-    <t>Desarrollo Vista Pagina Loggin</t>
-  </si>
-  <si>
     <t>Desarrollo Vista Pagina Carrito</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>Desarrollo de la Vista Registro</t>
+  </si>
+  <si>
+    <t>Desarrollo Vista Pagina Login</t>
   </si>
 </sst>
 </file>
@@ -781,18 +781,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -833,11 +821,810 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="51">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-240A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-240A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-240A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-240A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1030,793 +1817,6 @@
         <patternFill patternType="none"/>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9900"/>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="[$-240A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="[$-240A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9900"/>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="[$-240A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="[$-240A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1831,41 +1831,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F899EF04-071F-4438-9F03-C42B061D8F9E}" name="Tabla1" displayName="Tabla1" ref="A2:J10" totalsRowShown="0" headerRowDxfId="50" headerRowBorderDxfId="49" tableBorderDxfId="48" totalsRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F899EF04-071F-4438-9F03-C42B061D8F9E}" name="Tabla1" displayName="Tabla1" ref="A2:J10" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{66CC9B29-972E-440A-912D-BD4A014746AB}" name="Incr." dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{8DB82F78-68F3-42A2-850E-63D287D60F0F}" name="Start" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{F968D6EE-A810-4E1A-B390-2EB3FDF1FEBC}" name="Days" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{AAF044F0-1EF6-4F39-B0EC-7E4FF5284F1E}" name="End" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{43FD3FBC-D2AD-4693-A6D3-2D3C3CEA7764}" name="Estimated Size" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{845D7AAE-192D-4ACB-98F1-13E2AB396319}" name="Real Size" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{3A55337D-C59A-4152-AB89-7F958089BEB6}" name="Status" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{66CC9B29-972E-440A-912D-BD4A014746AB}" name="Incr." dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{8DB82F78-68F3-42A2-850E-63D287D60F0F}" name="Start" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{F968D6EE-A810-4E1A-B390-2EB3FDF1FEBC}" name="Days" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{AAF044F0-1EF6-4F39-B0EC-7E4FF5284F1E}" name="End" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{43FD3FBC-D2AD-4693-A6D3-2D3C3CEA7764}" name="Estimated Size" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{845D7AAE-192D-4ACB-98F1-13E2AB396319}" name="Real Size" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{3A55337D-C59A-4152-AB89-7F958089BEB6}" name="Status" dataDxfId="16"/>
     <tableColumn id="8" xr3:uid="{38918B64-CCE0-4636-A5E4-263FE5F24E44}" name="Release Date"/>
-    <tableColumn id="9" xr3:uid="{60143B17-7058-4AA2-BE5E-4B4A6B0F3F79}" name="Goal" dataDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{08E89F60-45A7-4FE5-84CF-07185CF17579}" name="% Esfuerzo vs Estimación" dataDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{60143B17-7058-4AA2-BE5E-4B4A6B0F3F79}" name="Goal" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{08E89F60-45A7-4FE5-84CF-07185CF17579}" name="% Esfuerzo vs Estimación" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6B9DA90-D87F-4F67-9EB9-B6BDCC070AB7}" name="Tabla2" displayName="Tabla2" ref="A13:K27" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6B9DA90-D87F-4F67-9EB9-B6BDCC070AB7}" name="Tabla2" displayName="Tabla2" ref="A13:K27" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{3F7F6DD2-6EA2-4440-BD0B-88E2A12AF313}" name="Sprint" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{62768372-7E11-44D1-A207-F692349A3997}" name="Start" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{3F7F6DD2-6EA2-4440-BD0B-88E2A12AF313}" name="Sprint" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{62768372-7E11-44D1-A207-F692349A3997}" name="Start" dataDxfId="9">
       <calculatedColumnFormula>IF(AND(B13&lt;&gt;"",C13&lt;&gt;"",C14&lt;&gt;""),B13+C13,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F25C110E-5E39-4470-8BC8-391189A23F6A}" name="Days" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{B5697784-C933-4A45-8BA8-617CDCABE74D}" name="End" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{F25C110E-5E39-4470-8BC8-391189A23F6A}" name="Days" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{B5697784-C933-4A45-8BA8-617CDCABE74D}" name="End" dataDxfId="7">
       <calculatedColumnFormula>IF(AND(B14&lt;&gt;"",C14&lt;&gt;""),B14+C14-1,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5518327B-86C2-485C-AF9A-553A341AB62F}" name="Estimated Size" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{8EE1AD7A-512C-42AD-9C83-F3DE570521F3}" name="Real Size" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{879F25EC-AE5A-403A-BB1E-715A98E973E5}" name="Status" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{35D9BAA4-D3E2-4602-BFEC-3D9FAF91D9FB}" name="Release Date" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{25759FDC-EAD4-41CE-B98D-B6CA5005C897}" name="Goal" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{767130C5-3778-4D2D-B165-AAC8557C9C26}" name="Increment" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{BB50C29E-17AE-4847-B617-C1464CB872F4}" name="% Error estimación" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{5518327B-86C2-485C-AF9A-553A341AB62F}" name="Estimated Size" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{8EE1AD7A-512C-42AD-9C83-F3DE570521F3}" name="Real Size" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{879F25EC-AE5A-403A-BB1E-715A98E973E5}" name="Status" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{35D9BAA4-D3E2-4602-BFEC-3D9FAF91D9FB}" name="Release Date" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{25759FDC-EAD4-41CE-B98D-B6CA5005C897}" name="Goal" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{767130C5-3778-4D2D-B165-AAC8557C9C26}" name="Increment" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{BB50C29E-17AE-4847-B617-C1464CB872F4}" name="% Error estimación" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2072,7 +2072,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2088,393 +2088,393 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="61" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="59">
+        <v>1</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="63">
+        <v>3</v>
+      </c>
+      <c r="E2" s="59">
+        <v>0</v>
+      </c>
+      <c r="F2" s="59">
+        <v>1</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="66"/>
+    </row>
+    <row r="3" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59">
+        <v>2</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="63">
+        <v>8</v>
+      </c>
+      <c r="E3" s="59">
+        <v>0</v>
+      </c>
+      <c r="F3" s="59">
+        <v>1</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="66"/>
+    </row>
+    <row r="4" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="59">
+        <v>3</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="63">
+        <v>20</v>
+      </c>
+      <c r="E4" s="59">
+        <v>0</v>
+      </c>
+      <c r="F4" s="59">
+        <v>1</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="66"/>
+    </row>
+    <row r="5" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="59">
+        <v>4</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="63">
+        <v>10</v>
+      </c>
+      <c r="E5" s="59">
+        <v>0</v>
+      </c>
+      <c r="F5" s="59">
+        <v>1</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="67"/>
+    </row>
+    <row r="6" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="59">
+        <v>5</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="63">
+        <v>13</v>
+      </c>
+      <c r="E6" s="59">
+        <v>0</v>
+      </c>
+      <c r="F6" s="59">
+        <v>1</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="67"/>
+    </row>
+    <row r="7" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="59">
+        <v>6</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="63">
+        <v>13</v>
+      </c>
+      <c r="E7" s="59">
+        <v>0</v>
+      </c>
+      <c r="F7" s="59">
+        <v>1</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="66"/>
+    </row>
+    <row r="8" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="59">
+        <v>7</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="63">
+        <v>13</v>
+      </c>
+      <c r="E8" s="59">
+        <v>0</v>
+      </c>
+      <c r="F8" s="59">
+        <v>1</v>
+      </c>
+      <c r="G8" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="66"/>
+    </row>
+    <row r="9" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="59">
+        <v>8</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="63">
+        <v>8</v>
+      </c>
+      <c r="E9" s="59">
+        <v>0</v>
+      </c>
+      <c r="F9" s="59">
+        <v>2</v>
+      </c>
+      <c r="G9" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="69"/>
+    </row>
+    <row r="10" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="60">
+        <v>9</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="63">
+        <v>10</v>
+      </c>
+      <c r="E10" s="60">
+        <v>1</v>
+      </c>
+      <c r="F10" s="60">
+        <v>1</v>
+      </c>
+      <c r="G10" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="62" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="65" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63">
+      <c r="H10" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="70" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="59">
+        <v>10</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="63">
+        <v>10</v>
+      </c>
+      <c r="E11" s="60">
         <v>1</v>
       </c>
-      <c r="B2" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="67">
-        <v>3</v>
-      </c>
-      <c r="E2" s="63">
-        <v>0</v>
-      </c>
-      <c r="F2" s="63">
+      <c r="F11" s="60">
         <v>1</v>
       </c>
-      <c r="G2" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="70"/>
-    </row>
-    <row r="3" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63">
-        <v>2</v>
-      </c>
-      <c r="B3" s="66" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="67">
-        <v>8</v>
-      </c>
-      <c r="E3" s="63">
-        <v>0</v>
-      </c>
-      <c r="F3" s="63">
+      <c r="G11" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="59">
+        <v>11</v>
+      </c>
+      <c r="B12" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="63">
+        <v>10</v>
+      </c>
+      <c r="E12" s="60">
         <v>1</v>
       </c>
-      <c r="G3" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="70"/>
-    </row>
-    <row r="4" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63">
-        <v>3</v>
-      </c>
-      <c r="B4" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="67">
-        <v>20</v>
-      </c>
-      <c r="E4" s="63">
-        <v>0</v>
-      </c>
-      <c r="F4" s="63">
+      <c r="F12" s="60">
         <v>1</v>
       </c>
-      <c r="G4" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="70"/>
-    </row>
-    <row r="5" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="63">
-        <v>4</v>
-      </c>
-      <c r="B5" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="67">
+      <c r="G12" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="69" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="60">
+        <v>12</v>
+      </c>
+      <c r="B13" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="63">
         <v>10</v>
       </c>
-      <c r="E5" s="63">
-        <v>0</v>
-      </c>
-      <c r="F5" s="63">
+      <c r="E13" s="60">
         <v>1</v>
       </c>
-      <c r="G5" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="69" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="71"/>
-    </row>
-    <row r="6" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="63">
-        <v>5</v>
-      </c>
-      <c r="B6" s="66" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="67">
+      <c r="F13" s="60">
+        <v>1</v>
+      </c>
+      <c r="G13" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="59">
         <v>13</v>
       </c>
-      <c r="E6" s="63">
-        <v>0</v>
-      </c>
-      <c r="F6" s="63">
+      <c r="B14" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="63">
+        <v>10</v>
+      </c>
+      <c r="E14" s="60">
         <v>1</v>
       </c>
-      <c r="G6" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="71"/>
-    </row>
-    <row r="7" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="63">
-        <v>6</v>
-      </c>
-      <c r="B7" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="67">
-        <v>13</v>
-      </c>
-      <c r="E7" s="63">
-        <v>0</v>
-      </c>
-      <c r="F7" s="63">
+      <c r="F14" s="60">
         <v>1</v>
       </c>
-      <c r="G7" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="70"/>
-    </row>
-    <row r="8" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="63">
-        <v>7</v>
-      </c>
-      <c r="B8" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="67">
-        <v>13</v>
-      </c>
-      <c r="E8" s="63">
-        <v>0</v>
-      </c>
-      <c r="F8" s="63">
-        <v>1</v>
-      </c>
-      <c r="G8" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="70"/>
-    </row>
-    <row r="9" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="63">
-        <v>8</v>
-      </c>
-      <c r="B9" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="67">
-        <v>8</v>
-      </c>
-      <c r="E9" s="63">
-        <v>0</v>
-      </c>
-      <c r="F9" s="63">
-        <v>2</v>
-      </c>
-      <c r="G9" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="73"/>
-    </row>
-    <row r="10" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="64">
-        <v>9</v>
-      </c>
-      <c r="B10" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="67">
-        <v>10</v>
-      </c>
-      <c r="E10" s="64">
-        <v>1</v>
-      </c>
-      <c r="F10" s="64">
-        <v>1</v>
-      </c>
-      <c r="G10" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="74" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="63">
-        <v>10</v>
-      </c>
-      <c r="B11" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="67">
-        <v>10</v>
-      </c>
-      <c r="E11" s="64">
-        <v>1</v>
-      </c>
-      <c r="F11" s="64">
-        <v>1</v>
-      </c>
-      <c r="G11" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="75" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="63">
-        <v>11</v>
-      </c>
-      <c r="B12" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="67">
-        <v>10</v>
-      </c>
-      <c r="E12" s="64">
-        <v>1</v>
-      </c>
-      <c r="F12" s="64">
-        <v>1</v>
-      </c>
-      <c r="G12" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="72" t="s">
+      <c r="G14" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="71" t="s">
         <v>63</v>
-      </c>
-      <c r="I12" s="73" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="64">
-        <v>12</v>
-      </c>
-      <c r="B13" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="67">
-        <v>10</v>
-      </c>
-      <c r="E13" s="64">
-        <v>1</v>
-      </c>
-      <c r="F13" s="64">
-        <v>1</v>
-      </c>
-      <c r="G13" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" s="75" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="63">
-        <v>13</v>
-      </c>
-      <c r="B14" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="67">
-        <v>10</v>
-      </c>
-      <c r="E14" s="64">
-        <v>1</v>
-      </c>
-      <c r="F14" s="64">
-        <v>1</v>
-      </c>
-      <c r="G14" s="68" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="I14" s="75" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2508,18 +2508,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:26" s="53" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
@@ -2780,19 +2780,19 @@
       <c r="J11" s="35"/>
     </row>
     <row r="12" spans="1:26" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
     </row>
     <row r="13" spans="1:26" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="48" t="s">
@@ -3294,12 +3294,12 @@
       <c r="L29" s="47"/>
     </row>
     <row r="30" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="61" t="s">
+      <c r="A30" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
       <c r="E30" s="56" t="e">
         <f>SUMIF(#REF!,"",#REF!)-SUMIF(#REF!,"Removed",#REF!)</f>
         <v>#REF!</v>
@@ -3310,12 +3310,12 @@
       <c r="I30" s="43"/>
     </row>
     <row r="31" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
       <c r="E31" s="56">
         <f>SUM(E14:E29)</f>
         <v>36.300000000000004</v>
@@ -6247,122 +6247,122 @@
     <mergeCell ref="A30:D30"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:I8 E4:F8 E30:F31 A3:D8 F5:I5">
-    <cfRule type="expression" dxfId="23" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="13" stopIfTrue="1">
       <formula>$G2="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I8 E4:F8 E30:F31 A3:D8 F5:I5">
-    <cfRule type="expression" dxfId="22" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="14" stopIfTrue="1">
       <formula>$G2="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G8 G14:G23 G29">
-    <cfRule type="expression" dxfId="21" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="15" stopIfTrue="1">
       <formula>$G3="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G8 H14:I16 H23:I23 I17:I21 G14:G23 H15:H22 G29:I29">
-    <cfRule type="expression" dxfId="20" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="16" stopIfTrue="1">
       <formula>$G3="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G8 G14:G23 G29">
-    <cfRule type="cellIs" dxfId="19" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Unplanned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E4 F3:F7 H3:H7 H14:I16 H23:I23 H15:H22 B14:F23 H29:I29 A29:F29">
-    <cfRule type="expression" dxfId="18" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="18" stopIfTrue="1">
       <formula>OR($G3="Planned",$G3="Unplanned")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E4 F3:F7 H3:H7 B14:F23 A29:F29">
-    <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="19" stopIfTrue="1">
       <formula>$G3="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B23">
-    <cfRule type="expression" dxfId="16" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="20" stopIfTrue="1">
       <formula>$G14="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B23">
-    <cfRule type="expression" dxfId="15" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="21" stopIfTrue="1">
       <formula>$G14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B23">
-    <cfRule type="expression" dxfId="14" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="22" stopIfTrue="1">
       <formula>$G14="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B23">
-    <cfRule type="expression" dxfId="13" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="23" stopIfTrue="1">
       <formula>$G14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:D23">
-    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="24" stopIfTrue="1">
       <formula>$G14="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:D23">
-    <cfRule type="expression" dxfId="11" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="25" stopIfTrue="1">
       <formula>$G14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:I21">
-    <cfRule type="expression" dxfId="10" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="34" stopIfTrue="1">
       <formula>OR($G17="Planned",$G17="Unplanned")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:J10">
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="11" stopIfTrue="1">
       <formula>$G9="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:J10">
-    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="12" stopIfTrue="1">
       <formula>$G9="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:J9">
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="9" stopIfTrue="1">
       <formula>$G8="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:J9">
-    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="10" stopIfTrue="1">
       <formula>$G8="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:J11">
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="7" stopIfTrue="1">
       <formula>$G10="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:J11">
-    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="8" stopIfTrue="1">
       <formula>$G10="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A23">
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="5" stopIfTrue="1">
       <formula>OR($G14="Planned",$G14="Unplanned")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:K28">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="1" stopIfTrue="1">
       <formula>OR($G24="Planned",$G24="Unplanned")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A23">
-    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="6" stopIfTrue="1">
       <formula>$G14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:K28">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="2" stopIfTrue="1">
       <formula>$G24="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>